<commit_message>
connected gui to logic
</commit_message>
<xml_diff>
--- a/Data/Exports/Schueler_Zuweisungen.xlsx
+++ b/Data/Exports/Schueler_Zuweisungen.xlsx
@@ -1319,7 +1319,7 @@
         <v>146</v>
       </c>
       <c r="D6">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1419,7 +1419,7 @@
         <v>147</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1519,7 +1519,7 @@
         <v>148</v>
       </c>
       <c r="D16">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1619,7 +1619,7 @@
         <v>149</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -1719,7 +1719,7 @@
         <v>150</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E26">
         <v>5</v>
@@ -1919,7 +1919,7 @@
         <v>152</v>
       </c>
       <c r="D36">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -2019,7 +2019,7 @@
         <v>153</v>
       </c>
       <c r="D41">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E41">
         <v>5</v>
@@ -2319,7 +2319,7 @@
         <v>156</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E56">
         <v>5</v>
@@ -2799,10 +2799,10 @@
         <v>161</v>
       </c>
       <c r="D80">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E80">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F80" t="s">
         <v>276</v>
@@ -2819,10 +2819,10 @@
         <v>161</v>
       </c>
       <c r="D81">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E81">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F81" t="s">
         <v>276</v>
@@ -2919,7 +2919,7 @@
         <v>162</v>
       </c>
       <c r="D86">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E86">
         <v>5</v>
@@ -3019,7 +3019,7 @@
         <v>163</v>
       </c>
       <c r="D91">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E91">
         <v>3</v>
@@ -3119,7 +3119,7 @@
         <v>164</v>
       </c>
       <c r="D96">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E96">
         <v>2</v>
@@ -3219,7 +3219,7 @@
         <v>165</v>
       </c>
       <c r="D101">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E101">
         <v>3</v>
@@ -3519,7 +3519,7 @@
         <v>168</v>
       </c>
       <c r="D116">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E116">
         <v>5</v>
@@ -3619,7 +3619,7 @@
         <v>17</v>
       </c>
       <c r="D121">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E121">
         <v>5</v>
@@ -3719,7 +3719,7 @@
         <v>169</v>
       </c>
       <c r="D126">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E126">
         <v>5</v>
@@ -3819,7 +3819,7 @@
         <v>170</v>
       </c>
       <c r="D131">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -4019,7 +4019,7 @@
         <v>172</v>
       </c>
       <c r="D141">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E141">
         <v>3</v>
@@ -4119,7 +4119,7 @@
         <v>173</v>
       </c>
       <c r="D146">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E146">
         <v>2</v>
@@ -4199,7 +4199,7 @@
         <v>174</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -4219,7 +4219,7 @@
         <v>174</v>
       </c>
       <c r="D151">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E151">
         <v>2</v>
@@ -4619,7 +4619,7 @@
         <v>178</v>
       </c>
       <c r="D171">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -4719,7 +4719,7 @@
         <v>179</v>
       </c>
       <c r="D176">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E176">
         <v>2</v>
@@ -4819,7 +4819,7 @@
         <v>180</v>
       </c>
       <c r="D181">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E181">
         <v>5</v>
@@ -5199,10 +5199,10 @@
         <v>184</v>
       </c>
       <c r="D200">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E200">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F200" t="s">
         <v>276</v>
@@ -5219,10 +5219,10 @@
         <v>184</v>
       </c>
       <c r="D201">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E201">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F201" t="s">
         <v>276</v>
@@ -5319,7 +5319,7 @@
         <v>185</v>
       </c>
       <c r="D206">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E206">
         <v>5</v>
@@ -5379,7 +5379,7 @@
         <v>186</v>
       </c>
       <c r="D209">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -5399,10 +5399,10 @@
         <v>186</v>
       </c>
       <c r="D210">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E210">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F210" t="s">
         <v>276</v>
@@ -5419,10 +5419,10 @@
         <v>186</v>
       </c>
       <c r="D211">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E211">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F211" t="s">
         <v>276</v>
@@ -5819,7 +5819,7 @@
         <v>190</v>
       </c>
       <c r="D231">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E231">
         <v>5</v>
@@ -6019,7 +6019,7 @@
         <v>192</v>
       </c>
       <c r="D241">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E241">
         <v>5</v>
@@ -6319,7 +6319,7 @@
         <v>195</v>
       </c>
       <c r="D256">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E256">
         <v>2</v>
@@ -6499,7 +6499,7 @@
         <v>197</v>
       </c>
       <c r="D265">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E265">
         <v>4</v>
@@ -6519,7 +6519,7 @@
         <v>197</v>
       </c>
       <c r="D266">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E266">
         <v>2</v>
@@ -6619,7 +6619,7 @@
         <v>198</v>
       </c>
       <c r="D271">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E271">
         <v>5</v>
@@ -6719,7 +6719,7 @@
         <v>199</v>
       </c>
       <c r="D276">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E276">
         <v>3</v>
@@ -6819,7 +6819,7 @@
         <v>200</v>
       </c>
       <c r="D281">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E281">
         <v>5</v>
@@ -6899,10 +6899,10 @@
         <v>201</v>
       </c>
       <c r="D285">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E285">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F285" t="s">
         <v>276</v>
@@ -6919,10 +6919,10 @@
         <v>201</v>
       </c>
       <c r="D286">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E286">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F286" t="s">
         <v>276</v>
@@ -7019,7 +7019,7 @@
         <v>202</v>
       </c>
       <c r="D291">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E291">
         <v>4</v>
@@ -7119,7 +7119,7 @@
         <v>203</v>
       </c>
       <c r="D296">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E296">
         <v>5</v>
@@ -7319,7 +7319,7 @@
         <v>205</v>
       </c>
       <c r="D306">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E306">
         <v>1</v>
@@ -8319,7 +8319,7 @@
         <v>215</v>
       </c>
       <c r="D356">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E356">
         <v>2</v>
@@ -8519,7 +8519,7 @@
         <v>165</v>
       </c>
       <c r="D366">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E366">
         <v>5</v>
@@ -8699,10 +8699,10 @@
         <v>218</v>
       </c>
       <c r="D375">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E375">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F375" t="s">
         <v>276</v>
@@ -8719,10 +8719,10 @@
         <v>218</v>
       </c>
       <c r="D376">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E376">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F376" t="s">
         <v>276</v>
@@ -9019,7 +9019,7 @@
         <v>118</v>
       </c>
       <c r="D391">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E391">
         <v>5</v>
@@ -9119,7 +9119,7 @@
         <v>221</v>
       </c>
       <c r="D396">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E396">
         <v>2</v>
@@ -9319,7 +9319,7 @@
         <v>223</v>
       </c>
       <c r="D406">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E406">
         <v>2</v>
@@ -9619,7 +9619,7 @@
         <v>226</v>
       </c>
       <c r="D421">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E421">
         <v>3</v>
@@ -9719,7 +9719,7 @@
         <v>181</v>
       </c>
       <c r="D426">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E426">
         <v>2</v>
@@ -9819,7 +9819,7 @@
         <v>227</v>
       </c>
       <c r="D431">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E431">
         <v>3</v>
@@ -9919,7 +9919,7 @@
         <v>228</v>
       </c>
       <c r="D436">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E436">
         <v>5</v>
@@ -10019,7 +10019,7 @@
         <v>229</v>
       </c>
       <c r="D441">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E441">
         <v>5</v>
@@ -10519,7 +10519,7 @@
         <v>234</v>
       </c>
       <c r="D466">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E466">
         <v>3</v>
@@ -10719,7 +10719,7 @@
         <v>236</v>
       </c>
       <c r="D476">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E476">
         <v>2</v>
@@ -10919,7 +10919,7 @@
         <v>238</v>
       </c>
       <c r="D486">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E486">
         <v>2</v>
@@ -11019,7 +11019,7 @@
         <v>239</v>
       </c>
       <c r="D491">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E491">
         <v>2</v>
@@ -11119,7 +11119,7 @@
         <v>240</v>
       </c>
       <c r="D496">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E496">
         <v>5</v>
@@ -11299,10 +11299,10 @@
         <v>242</v>
       </c>
       <c r="D505">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E505">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F505" t="s">
         <v>276</v>
@@ -11319,10 +11319,10 @@
         <v>242</v>
       </c>
       <c r="D506">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E506">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F506" t="s">
         <v>276</v>
@@ -11399,7 +11399,7 @@
         <v>243</v>
       </c>
       <c r="D510">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E510">
         <v>4</v>
@@ -11419,7 +11419,7 @@
         <v>243</v>
       </c>
       <c r="D511">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E511">
         <v>3</v>
@@ -11519,7 +11519,7 @@
         <v>244</v>
       </c>
       <c r="D516">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E516">
         <v>5</v>
@@ -11599,7 +11599,7 @@
         <v>245</v>
       </c>
       <c r="D520">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E520">
         <v>3</v>
@@ -11619,7 +11619,7 @@
         <v>245</v>
       </c>
       <c r="D521">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E521">
         <v>4</v>
@@ -12119,7 +12119,7 @@
         <v>250</v>
       </c>
       <c r="D546">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E546">
         <v>2</v>
@@ -12319,7 +12319,7 @@
         <v>252</v>
       </c>
       <c r="D556">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E556">
         <v>5</v>
@@ -12419,7 +12419,7 @@
         <v>253</v>
       </c>
       <c r="D561">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E561">
         <v>5</v>
@@ -12699,10 +12699,10 @@
         <v>256</v>
       </c>
       <c r="D575">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E575">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F575" t="s">
         <v>276</v>
@@ -12719,10 +12719,10 @@
         <v>256</v>
       </c>
       <c r="D576">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E576">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F576" t="s">
         <v>276</v>
@@ -12819,7 +12819,7 @@
         <v>257</v>
       </c>
       <c r="D581">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E581">
         <v>4</v>
@@ -12919,7 +12919,7 @@
         <v>258</v>
       </c>
       <c r="D586">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E586">
         <v>4</v>
@@ -13019,7 +13019,7 @@
         <v>259</v>
       </c>
       <c r="D591">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E591">
         <v>3</v>
@@ -13519,7 +13519,7 @@
         <v>263</v>
       </c>
       <c r="D616">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E616">
         <v>5</v>
@@ -13619,7 +13619,7 @@
         <v>264</v>
       </c>
       <c r="D621">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E621">
         <v>5</v>
@@ -13719,7 +13719,7 @@
         <v>265</v>
       </c>
       <c r="D626">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E626">
         <v>3</v>
@@ -13819,7 +13819,7 @@
         <v>266</v>
       </c>
       <c r="D631">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E631">
         <v>5</v>
@@ -13919,7 +13919,7 @@
         <v>267</v>
       </c>
       <c r="D636">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E636">
         <v>5</v>
@@ -14019,7 +14019,7 @@
         <v>268</v>
       </c>
       <c r="D641">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E641">
         <v>2</v>
@@ -14119,7 +14119,7 @@
         <v>20</v>
       </c>
       <c r="D646">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E646">
         <v>5</v>
@@ -14202,7 +14202,7 @@
         <v>17</v>
       </c>
       <c r="E650">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F650" t="s">
         <v>276</v>
@@ -14219,10 +14219,10 @@
         <v>269</v>
       </c>
       <c r="D651">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E651">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F651" t="s">
         <v>276</v>
@@ -14319,7 +14319,7 @@
         <v>270</v>
       </c>
       <c r="D656">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E656">
         <v>4</v>
@@ -14419,7 +14419,7 @@
         <v>271</v>
       </c>
       <c r="D661">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E661">
         <v>3</v>
@@ -14519,7 +14519,7 @@
         <v>272</v>
       </c>
       <c r="D666">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E666">
         <v>1</v>
@@ -14539,10 +14539,10 @@
         <v>273</v>
       </c>
       <c r="D667">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E667">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F667" t="s">
         <v>276</v>
@@ -14559,10 +14559,10 @@
         <v>273</v>
       </c>
       <c r="D668">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E668">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F668" t="s">
         <v>276</v>
@@ -14582,7 +14582,7 @@
         <v>22</v>
       </c>
       <c r="E669">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F669" t="s">
         <v>276</v>
@@ -14619,10 +14619,10 @@
         <v>273</v>
       </c>
       <c r="D671">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E671">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F671" t="s">
         <v>276</v>
@@ -14639,10 +14639,10 @@
         <v>274</v>
       </c>
       <c r="D672">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E672">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F672" t="s">
         <v>276</v>
@@ -14659,10 +14659,10 @@
         <v>274</v>
       </c>
       <c r="D673">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E673">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F673" t="s">
         <v>276</v>
@@ -14679,10 +14679,10 @@
         <v>274</v>
       </c>
       <c r="D674">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E674">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F674" t="s">
         <v>276</v>
@@ -14699,10 +14699,10 @@
         <v>274</v>
       </c>
       <c r="D675">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E675">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F675" t="s">
         <v>276</v>
@@ -14719,10 +14719,10 @@
         <v>274</v>
       </c>
       <c r="D676">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E676">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F676" t="s">
         <v>276</v>

</xml_diff>